<commit_message>
ajout des fichiers de production
</commit_message>
<xml_diff>
--- a/BOMs/BOM_globale.xlsx
+++ b/BOMs/BOM_globale.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="160">
   <si>
     <t>Mouser</t>
   </si>
@@ -552,6 +552,12 @@
   </si>
   <si>
     <t>Gain</t>
+  </si>
+  <si>
+    <t>https://fr.farnell.com/bak/lp-402025-is-3/batterie-lithium-pol-3-7v-165/dp/2077885</t>
+  </si>
+  <si>
+    <t>Batterie Li Poly</t>
   </si>
 </sst>
 </file>
@@ -734,6 +740,12 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -762,12 +774,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -835,14 +841,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.42928455818022748"/>
-          <c:y val="0"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -875,7 +874,7 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:doughnutChart>
+      <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
@@ -940,633 +939,43 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="11"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="12"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="13"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="15"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="16"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="17"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="18"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="19"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="20"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="21"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="22"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="23"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="24"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="25"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="26"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="27"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="28"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="29"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="30"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="31"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="32"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="33"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="34"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>ele!$A$60:$D$60</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>total IC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>total Connector</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>total Passiv</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>total HMI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ele!$M$5:$M$39</c:f>
+              <c:f>ele!$A$62:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.1476125563615911</c:v>
+                  <c:v>40.718413355211524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5023116593424399</c:v>
+                  <c:v>6.3613231552162848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.613357101322173</c:v>
+                  <c:v>1.5818093901849339</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1943509718501852E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.3354908820529437E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.20328303289705729</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.1609868163922856</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.64583472350647742</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0533540508851034</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.29789424515981427</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3607809118900316</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.73162826611250387</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.86031858002154371</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0485877429625463</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.9560355757223329</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.54812541109405821</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.79597342306702379</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.7888239611831882</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.1466878926246151</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14.012945292317664</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.20328303289705729</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.3401142007378239E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0485877429625463E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.4546485801168698</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.8616340810081686</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.1915769806392571</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>12.034927504456496</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.6691324366319362</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>6.1962002993241372</c:v>
+                  <c:v>6.1155897996876796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1582,8 +991,7 @@
           <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
-        <c:holeSize val="75"/>
-      </c:doughnutChart>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1594,6 +1002,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1606,7 +1015,7 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr rtl="0">
+          <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -2223,20 +1632,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2255,15 +1664,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SKY_R" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SKY_G" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SKY_G_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SKY_R" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2532,7 +1941,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:H2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,46 +1962,45 @@
       <c r="C1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="16" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>mec!F3</f>
-        <v>46.41</v>
+        <v>25</v>
       </c>
       <c r="B2" s="8">
-        <f>ele!B57</f>
-        <v>41.961200000000005</v>
+        <f>ele!B58</f>
+        <v>50.461200000000005</v>
       </c>
       <c r="C2" s="8">
         <f>B2+A2</f>
-        <v>88.371200000000002</v>
+        <v>75.461200000000005</v>
       </c>
       <c r="D2">
         <f>C2+B5</f>
-        <v>123.3712</v>
+        <v>110.46120000000001</v>
       </c>
       <c r="E2">
         <f>5</f>
         <v>5</v>
       </c>
       <c r="F2">
-        <f>E2*D2</f>
-        <v>616.85599999999999</v>
+        <f>E2*C2</f>
+        <v>377.30600000000004</v>
       </c>
       <c r="G2">
         <f>E2*130</f>
@@ -2600,14 +2008,14 @@
       </c>
       <c r="H2">
         <f>G2-F2</f>
-        <v>33.144000000000005</v>
+        <v>272.69399999999996</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="17" t="s">
         <v>147</v>
       </c>
       <c r="C4" t="s">
@@ -2626,8 +2034,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2640,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,42 +2061,44 @@
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2724,23 +2134,23 @@
       </c>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2780,11 +2190,11 @@
         <v>123</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M20" si="0">(K5/$B$57)*100</f>
-        <v>5.1476125563615911</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M5:M20" si="0">(K5/$B$58)*100</f>
+        <v>4.2805165156595564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2825,10 +2235,10 @@
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>2.5023116593424399</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2.0808066395567288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -2869,10 +2279,10 @@
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>19.613357101322173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>16.309560612906548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2912,10 +2322,10 @@
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>4.1943509718501852E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.4878282720188974E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -2955,10 +2365,10 @@
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>2.3354908820529437E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.9420861969196131E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -2998,10 +2408,10 @@
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>0.20328303289705729</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.16904076795637044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -3042,10 +2452,10 @@
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>4.1609868163922856</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.4600841834914742</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -3086,10 +2496,10 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0.64583472350647742</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.53704628506654617</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -3130,10 +2540,10 @@
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>1.0533540508851034</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.87592050922292775</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -3174,10 +2584,10 @@
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0.29789424515981427</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.24771507613770577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -3218,10 +2628,10 @@
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>1.3607809118900316</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.13156246779704</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
@@ -3262,7 +2672,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0.73162826611250387</v>
+        <v>0.60838822699420536</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3306,7 +2716,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>0.86031858002154371</v>
+        <v>0.7154011398856942</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -3349,7 +2759,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>1.0485877429625463</v>
+        <v>0.87195706800472439</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3392,7 +2802,7 @@
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>3.9560355757223329</v>
+        <v>3.2896562111087322</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -3436,23 +2846,23 @@
       </c>
       <c r="M20">
         <f t="shared" si="0"/>
-        <v>0.54812541109405821</v>
+        <v>0.45579574009337859</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -3505,8 +2915,8 @@
         <v>123</v>
       </c>
       <c r="M23">
-        <f t="shared" ref="M23:M29" si="5">(K23/$B$57)*100</f>
-        <v>0.79597342306702379</v>
+        <f t="shared" ref="M23:M29" si="5">(K23/$B$58)*100</f>
+        <v>0.66189468343994984</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -3548,7 +2958,7 @@
       </c>
       <c r="M24">
         <f t="shared" si="5"/>
-        <v>0.7888239611831882</v>
+        <v>0.65594952161264497</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3590,7 +3000,7 @@
       </c>
       <c r="M25">
         <f t="shared" si="5"/>
-        <v>4.1466878926246151</v>
+        <v>3.4481938598368642</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -3634,7 +3044,7 @@
       </c>
       <c r="M26">
         <f t="shared" si="5"/>
-        <v>14.012945292317664</v>
+        <v>11.65251718151768</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -3677,7 +3087,7 @@
       </c>
       <c r="M27">
         <f t="shared" si="5"/>
-        <v>0.20328303289705729</v>
+        <v>0.16904076795637044</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -3721,7 +3131,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="5"/>
-        <v>7.3401142007378239E-2</v>
+        <v>6.1036994760330705E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -3765,23 +3175,23 @@
       </c>
       <c r="M29">
         <f t="shared" si="5"/>
-        <v>1.0485877429625463E-2</v>
+        <v>8.7195706800472436E-3</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -3818,8 +3228,8 @@
         <v>127</v>
       </c>
       <c r="M31">
-        <f>(K31/$B$57)*100</f>
-        <v>2.4546485801168698</v>
+        <f>(K31/$B$58)*100</f>
+        <v>2.0411722273746955</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3857,8 +3267,8 @@
         <v>123</v>
       </c>
       <c r="M32">
-        <f>(K32/$B$57)*100</f>
-        <v>4.8616340810081686</v>
+        <f>(K32/$B$58)*100</f>
+        <v>4.0427100425673581</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3896,8 +3306,8 @@
         <v>125</v>
       </c>
       <c r="M33">
-        <f>(K33/$B$57)*100</f>
-        <v>1.1915769806392571</v>
+        <f>(K33/$B$58)*100</f>
+        <v>0.99086030455082308</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3924,145 +3334,159 @@
         <v>127</v>
       </c>
       <c r="M34">
-        <f>(K34/$B$57)*100</f>
-        <v>12.034927504456496</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="24" t="s">
+        <f>(K34/$B$58)*100</f>
+        <v>10.007689075963313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="J35" s="3">
+        <v>15.14</v>
+      </c>
+      <c r="K35" s="3">
+        <f>J35*C35</f>
+        <v>15.14</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="M35">
+        <f>(K35/$B$58)*100</f>
+        <v>30.003250021798927</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A36" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="25">
         <v>1.1200000000000001</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="M37">
-        <f>(A37/$B$57)*100</f>
-        <v>2.6691324366319362</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="M38">
+        <f>(A38/$B$58)*100</f>
+        <v>2.219527082193844</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="25">
         <v>2.6</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="M39">
-        <f>(A39/$B$57)*100</f>
-        <v>6.1962002993241372</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="M40">
+        <f>(A40/$B$58)*100</f>
+        <v>5.152473583664281</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B49" s="20">
-        <f>SUM(K23:K33)</f>
-        <v>11.9755</v>
-      </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B50" s="20">
-        <v>1.8</v>
-      </c>
-      <c r="C50" s="20"/>
+        <v>119</v>
+      </c>
+      <c r="B50" s="22">
+        <f>SUM(K23:K29)</f>
+        <v>8.4055</v>
+      </c>
+      <c r="C50" s="22"/>
       <c r="D50" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="20">
-        <f>B50+B49</f>
-        <v>13.775500000000001</v>
-      </c>
-      <c r="C51" s="20"/>
+        <v>120</v>
+      </c>
+      <c r="B51" s="22">
+        <v>1.8</v>
+      </c>
+      <c r="C51" s="22"/>
       <c r="D51" s="9" t="s">
         <v>79</v>
       </c>
@@ -4072,120 +3496,137 @@
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="22">
+        <f>B51+B50</f>
+        <v>10.205500000000001</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B54" s="20">
         <f>SUM(K5:K20)</f>
         <v>17.705700000000004</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B54" s="18">
-        <v>1.86</v>
-      </c>
-      <c r="C54" s="19"/>
+      <c r="C54" s="21"/>
       <c r="D54" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" s="18">
-        <f>B54+B53</f>
-        <v>19.565700000000003</v>
-      </c>
-      <c r="C55" s="19"/>
+        <v>122</v>
+      </c>
+      <c r="B55" s="20">
+        <v>1.86</v>
+      </c>
+      <c r="C55" s="21"/>
       <c r="D55" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="20">
+        <f>B55+B54</f>
+        <v>19.565700000000003</v>
+      </c>
+      <c r="C56" s="21"/>
+      <c r="D56" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B56" s="21">
-        <f>SUM(K31:K34)</f>
-        <v>8.620000000000001</v>
-      </c>
-      <c r="C56" s="22"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="B57" s="23">
+        <f>SUM(K33:K35)</f>
+        <v>20.69</v>
+      </c>
+      <c r="C57" s="24"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B57" s="20">
-        <f>B55+B51+B56</f>
-        <v>41.961200000000005</v>
-      </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="9" t="s">
+      <c r="B58" s="22">
+        <f>B56+B52+B57</f>
+        <v>50.461200000000005</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="D58" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>128</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>129</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>130</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <f>K5+K12+K15+K23+K24+K25+K32</f>
-        <v>7.4470000000000001</v>
-      </c>
-      <c r="B60">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f>K5+K12+K15+K23+K24+K25+K35</f>
+        <v>20.547000000000001</v>
+      </c>
+      <c r="B61">
         <f>K33+K19+K6</f>
         <v>3.21</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <f>K29+K28+K27+K18+K14+K10+K9+K8</f>
         <v>0.79820000000000002</v>
       </c>
-      <c r="D60">
-        <f>K31+K20+K17+K16+K13+K11</f>
-        <v>4.1159999999999997</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f>(A60/B57)*100</f>
-        <v>17.747347549641095</v>
-      </c>
-      <c r="B61">
-        <f>(B60/B57)*100</f>
-        <v>7.649924215704031</v>
-      </c>
-      <c r="C61">
-        <f>(C60/B57)*100</f>
-        <v>1.9022334918925101</v>
-      </c>
       <c r="D61">
-        <f>(D60/B57)*100</f>
-        <v>9.8090617046223638</v>
+        <f>K20+K17+K16+K13+K11</f>
+        <v>3.0859999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f>(A61/B58)*100</f>
+        <v>40.718413355211524</v>
+      </c>
+      <c r="B62">
+        <f>(B61/B58)*100</f>
+        <v>6.3613231552162848</v>
+      </c>
+      <c r="C62">
+        <f>(C61/B58)*100</f>
+        <v>1.5818093901849339</v>
+      </c>
+      <c r="D62">
+        <f>(D61/B58)*100</f>
+        <v>6.1155897996876796</v>
       </c>
     </row>
   </sheetData>
@@ -4194,22 +3635,22 @@
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="A30:K30"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:K36"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B58:C58"/>
     <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A37:K37"/>
     <mergeCell ref="A38:K38"/>
     <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="B56:C56"/>
     <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B49:C49"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <conditionalFormatting sqref="G22:I22">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
@@ -4261,10 +3702,11 @@
     <hyperlink ref="I27" r:id="rId38"/>
     <hyperlink ref="I18" r:id="rId39"/>
     <hyperlink ref="I33" r:id="rId40"/>
+    <hyperlink ref="I35" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId41"/>
-  <drawing r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
+  <drawing r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -4273,7 +3715,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4284,19 +3726,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="27" t="s">
         <v>99</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -4305,11 +3747,11 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="3" t="s">
         <v>145</v>
       </c>

</xml_diff>